<commit_message>
complete nodes and edges
</commit_message>
<xml_diff>
--- a/nodes-from-map-basic.xlsx
+++ b/nodes-from-map-basic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\school\cmsc204-final-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399A9ED8-BC37-46A2-80D5-1740260D5809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520E131E-C94F-41ED-BB7C-49FE20D93C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -955,7 +955,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>